<commit_message>
Automatische test-sync: 2025-08-02 00:03:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-02.xlsx
+++ b/logs/mail_log_2025-08-02.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -740,8 +740,64 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Testmail #13: Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedankt voor je interesse in de VentiQ-250. Helaas kan ik de datasheet niet direct via e-mail versturen, maar je kunt de datasheet vinden op onze website [link naar datasheet]. Mocht je nog vragen hebben of meer informatie nodig hebben, dan hoor ik het graag!
+Met vriendelijke groet,
+[Naam] 
+E-mailassistent van [Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-08-02 00:02:59</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -761,7 +817,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -769,17 +825,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -794,7 +850,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -824,6 +880,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-02 00:05:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-02.xlsx
+++ b/logs/mail_log_2025-08-02.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -796,8 +796,65 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Heb je de CE-certificaten van dit product?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Testmail #14: Heb je de CE-certificaten van dit product?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Geachte afzender,
+Dank u voor uw bericht. Helaas kan ik u op dit moment niet voorzien van de CE-certificaten van het genoemde product. Om u verder te helpen, zou u ons de naam van het specifieke product kunnen doorgeven, zodat we uw vraag nauwkeuriger kunnen beantwoorden.
+Ik kijk uit naar uw reactie.
+Met vriendelijke groet,
+[Naam]
+Nederlandse e-mailassistent</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-08-02 00:05:16</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -817,7 +874,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -825,17 +882,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -873,17 +930,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-02 00:08:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-02.xlsx
+++ b/logs/mail_log_2025-08-02.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -853,8 +853,63 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Testmail #15: Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedankt voor het verzenden van Testmail #15. In uw e-mail staat het verzoek om dit even neer te leggen bij Koen. Kunt u mij iets meer context geven over wat precies neergelegd moet worden bij Koen en waarom dat nodig is? Op die manier kan ik u beter helpen.
+Met vriendelijke groet,
+[Naam] - E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-08-02 00:07:56</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -874,7 +929,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -882,17 +937,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -907,7 +962,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -947,6 +1002,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-02 00:10:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-02.xlsx
+++ b/logs/mail_log_2025-08-02.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -908,8 +908,63 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Wil je dit even doorsturen?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Testmail #16: Wil je dit even doorsturen?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedankt voor je bericht. Het is helaas niet helemaal duidelijk wat je precies bedoelt met "Testmail #16: Wil je dit even doorsturen?". Zou je meer informatie kunnen geven over wat je wilt dat er wordt doorgestuurd en naar welk e-mailadres dit moet gebeuren?
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-08-02 00:10:07</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -929,7 +984,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -937,17 +992,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="J2:J6">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -995,17 +1050,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Intern verzoek / Actie voor medewerker</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-02 00:12:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-02.xlsx
+++ b/logs/mail_log_2025-08-02.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -963,8 +963,63 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Testmail #17: Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedank u voor uw e-mail. Ik bevestig graag de afspraak voor de demo bij Van Dijk op vrijdag om 11:00 uur.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-08-02 00:12:20</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -984,7 +1039,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -992,17 +1047,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J6">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1017,7 +1072,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1067,6 +1122,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-02 00:14:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-02.xlsx
+++ b/logs/mail_log_2025-08-02.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1018,8 +1018,60 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Testmail #18: Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-08-02 00:14:30</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1039,7 +1091,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1047,17 +1099,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="J2:J8">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1072,7 +1124,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1132,6 +1184,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-02 00:16:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-02.xlsx
+++ b/logs/mail_log_2025-08-02.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1070,8 +1070,64 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Testmail #19: Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Beste,
+Bedankt voor je e-mail. Het spijt me, maar ik heb geen verdere informatie over welke klant Jansen je bedoelt. Zou je meer context kunnen geven, zodat ik je beter kan helpen?
+Met vriendelijke groet,
+[Je naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-08-02 00:16:41</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1091,7 +1147,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1099,17 +1155,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J8">
+  <conditionalFormatting sqref="J2:J9">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1147,17 +1203,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Intern verzoek / Actie voor medewerker</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-02 00:19:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-02.xlsx
+++ b/logs/mail_log_2025-08-02.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$6</f>
+              <f>'Dashboard'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$6</f>
+              <f>'Dashboard'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1126,8 +1126,60 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Testmail #20: Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-08-02 00:18:52</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1147,7 +1199,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1155,17 +1207,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H2:H10">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J9">
+  <conditionalFormatting sqref="J2:J10">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1180,7 +1232,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1250,6 +1302,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>